<commit_message>
todo lo que queda
</commit_message>
<xml_diff>
--- a/ESTADISTICAS/Datos almacenados/Prueba2_recepcion_guardado_2estaciones_conreset.xlsx
+++ b/ESTADISTICAS/Datos almacenados/Prueba2_recepcion_guardado_2estaciones_conreset.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dani\Documents\2023-24\TFG\TFG_DANI_ANTO\ESTADISTICAS\Datos almacenados\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B271DB76-05E6-4141-B570-96839F733CAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21775FE7-DCBF-4DD7-A670-88478B587A96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="770" firstSheet="2" activeTab="5" xr2:uid="{0941D127-4EB4-43CB-A300-BE0423F61BB5}"/>
+    <workbookView minimized="1" xWindow="690" yWindow="690" windowWidth="7500" windowHeight="6000" tabRatio="770" activeTab="2" xr2:uid="{0941D127-4EB4-43CB-A300-BE0423F61BB5}"/>
   </bookViews>
   <sheets>
     <sheet name="Estacion1_6_12_2023" sheetId="1" r:id="rId1"/>
@@ -38,6 +38,23 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="4">
+  <si>
+    <t>Err todo 0s</t>
+  </si>
+  <si>
+    <t>Error Temp</t>
+  </si>
+  <si>
+    <t>Error Hum</t>
+  </si>
+  <si>
+    <t>Error tot</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -29103,15 +29120,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>180975</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>128587</xdr:rowOff>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>180975</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>14287</xdr:rowOff>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -29186,16 +29203,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>180975</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>128587</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>123825</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>180975</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>14287</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>123825</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -29267,9 +29284,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - Tema de 2022">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -29307,7 +29324,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -29413,7 +29430,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -29555,7 +29572,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -29563,15 +29580,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2634137E-43E4-465C-97F8-F10DB7750AE5}">
-  <dimension ref="A1:F216"/>
+  <dimension ref="A1:L216"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+      <selection activeCell="I16" sqref="I16:L17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="1">
         <v>45266</v>
       </c>
@@ -29591,7 +29608,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>45266</v>
       </c>
@@ -29611,7 +29628,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>45266</v>
       </c>
@@ -29631,7 +29648,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>45266</v>
       </c>
@@ -29651,7 +29668,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>45266</v>
       </c>
@@ -29671,7 +29688,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>45266</v>
       </c>
@@ -29691,7 +29708,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>45266</v>
       </c>
@@ -29711,7 +29728,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>45266</v>
       </c>
@@ -29731,7 +29748,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>45266</v>
       </c>
@@ -29751,7 +29768,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>45266</v>
       </c>
@@ -29771,7 +29788,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>45266</v>
       </c>
@@ -29791,7 +29808,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>45266</v>
       </c>
@@ -29811,7 +29828,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>45266</v>
       </c>
@@ -29831,7 +29848,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>45266</v>
       </c>
@@ -29851,7 +29868,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>45266</v>
       </c>
@@ -29871,7 +29888,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>45266</v>
       </c>
@@ -29890,8 +29907,20 @@
       <c r="F16">
         <v>9</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I16" t="s">
+        <v>0</v>
+      </c>
+      <c r="J16" t="s">
+        <v>1</v>
+      </c>
+      <c r="K16" t="s">
+        <v>2</v>
+      </c>
+      <c r="L16" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>45266</v>
       </c>
@@ -29910,8 +29939,24 @@
       <c r="F17">
         <v>9</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I17">
+        <f>COUNTIF(F1:F635,"0")</f>
+        <v>0</v>
+      </c>
+      <c r="J17">
+        <f>COUNTIF(C1:C635,"0")-I17</f>
+        <v>1</v>
+      </c>
+      <c r="K17">
+        <f>COUNTIF(D1:D635,"0")-I17</f>
+        <v>2</v>
+      </c>
+      <c r="L17">
+        <f>I17+K17</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>45266</v>
       </c>
@@ -29931,7 +29976,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>45266</v>
       </c>
@@ -29951,7 +29996,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>45266</v>
       </c>
@@ -29971,7 +30016,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>45266</v>
       </c>
@@ -29991,7 +30036,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>45266</v>
       </c>
@@ -30011,7 +30056,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>45266</v>
       </c>
@@ -30031,7 +30076,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>45266</v>
       </c>
@@ -30051,7 +30096,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>45266</v>
       </c>
@@ -30071,7 +30116,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>45266</v>
       </c>
@@ -30091,7 +30136,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>45266</v>
       </c>
@@ -30111,7 +30156,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>45266</v>
       </c>
@@ -30131,7 +30176,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>45266</v>
       </c>
@@ -30151,7 +30196,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>45266</v>
       </c>
@@ -30171,7 +30216,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>45266</v>
       </c>
@@ -30191,7 +30236,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>45266</v>
       </c>
@@ -33899,15 +33944,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB5FFFD5-8DDA-4AC5-A418-77532D651EB6}">
-  <dimension ref="A1:F215"/>
+  <dimension ref="A1:L215"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <selection activeCell="I16" sqref="I16:L17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="1">
         <v>45266</v>
       </c>
@@ -33927,7 +33972,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>45266</v>
       </c>
@@ -33947,7 +33992,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>45266</v>
       </c>
@@ -33967,7 +34012,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>45266</v>
       </c>
@@ -33987,7 +34032,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>45266</v>
       </c>
@@ -34007,7 +34052,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>45266</v>
       </c>
@@ -34027,7 +34072,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>45266</v>
       </c>
@@ -34047,7 +34092,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>45266</v>
       </c>
@@ -34067,7 +34112,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>45266</v>
       </c>
@@ -34087,7 +34132,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>45266</v>
       </c>
@@ -34107,7 +34152,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>45266</v>
       </c>
@@ -34127,7 +34172,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>45266</v>
       </c>
@@ -34147,7 +34192,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>45266</v>
       </c>
@@ -34167,7 +34212,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>45266</v>
       </c>
@@ -34187,7 +34232,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>45266</v>
       </c>
@@ -34207,7 +34252,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>45266</v>
       </c>
@@ -34226,8 +34271,20 @@
       <c r="F16">
         <v>9</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I16" t="s">
+        <v>0</v>
+      </c>
+      <c r="J16" t="s">
+        <v>1</v>
+      </c>
+      <c r="K16" t="s">
+        <v>2</v>
+      </c>
+      <c r="L16" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>45266</v>
       </c>
@@ -34246,8 +34303,24 @@
       <c r="F17">
         <v>9</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I17">
+        <f>COUNTIF(F1:F635,"0")</f>
+        <v>1</v>
+      </c>
+      <c r="J17">
+        <f>COUNTIF(C1:C635,"0")-I17</f>
+        <v>2</v>
+      </c>
+      <c r="K17">
+        <f>COUNTIF(D1:D635,"0")-I17</f>
+        <v>7</v>
+      </c>
+      <c r="L17">
+        <f>I17+K17</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>45266</v>
       </c>
@@ -34267,7 +34340,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>45266</v>
       </c>
@@ -34287,7 +34360,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>45266</v>
       </c>
@@ -34307,7 +34380,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>45266</v>
       </c>
@@ -34327,7 +34400,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>45266</v>
       </c>
@@ -34347,7 +34420,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>45266</v>
       </c>
@@ -34367,7 +34440,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>45266</v>
       </c>
@@ -34387,7 +34460,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>45266</v>
       </c>
@@ -34407,7 +34480,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>45266</v>
       </c>
@@ -34427,7 +34500,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>45266</v>
       </c>
@@ -34447,7 +34520,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>45266</v>
       </c>
@@ -34467,7 +34540,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>45266</v>
       </c>
@@ -34487,7 +34560,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>45266</v>
       </c>
@@ -34507,7 +34580,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>45266</v>
       </c>
@@ -34527,7 +34600,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>45266</v>
       </c>
@@ -38217,7 +38290,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05A1C15D-F8C2-4677-BF73-3BFD820956A9}">
   <dimension ref="A1:F211"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
@@ -42451,15 +42524,15 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3BEB0F7E-0F17-424B-B2B1-D78305F0FC2F}">
-  <dimension ref="A1:F436"/>
+  <dimension ref="A1:L436"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+      <selection activeCell="I16" sqref="I16:L17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="1">
         <v>45267</v>
       </c>
@@ -42479,7 +42552,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>45267</v>
       </c>
@@ -42499,7 +42572,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>45267</v>
       </c>
@@ -42519,7 +42592,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>45267</v>
       </c>
@@ -42539,7 +42612,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>45267</v>
       </c>
@@ -42559,7 +42632,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>45267</v>
       </c>
@@ -42579,7 +42652,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>45267</v>
       </c>
@@ -42599,7 +42672,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>45267</v>
       </c>
@@ -42619,7 +42692,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>45267</v>
       </c>
@@ -42639,7 +42712,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>45267</v>
       </c>
@@ -42659,7 +42732,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>45267</v>
       </c>
@@ -42679,7 +42752,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>45267</v>
       </c>
@@ -42699,7 +42772,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>45267</v>
       </c>
@@ -42719,7 +42792,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>45267</v>
       </c>
@@ -42739,7 +42812,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>45267</v>
       </c>
@@ -42759,7 +42832,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>45267</v>
       </c>
@@ -42778,8 +42851,20 @@
       <c r="F16">
         <v>9</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I16" t="s">
+        <v>0</v>
+      </c>
+      <c r="J16" t="s">
+        <v>1</v>
+      </c>
+      <c r="K16" t="s">
+        <v>2</v>
+      </c>
+      <c r="L16" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>45267</v>
       </c>
@@ -42798,8 +42883,24 @@
       <c r="F17">
         <v>9</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I17">
+        <f>COUNTIF(F1:F635,"0")</f>
+        <v>1</v>
+      </c>
+      <c r="J17">
+        <f>COUNTIF(C1:C635,"0")-I17</f>
+        <v>1</v>
+      </c>
+      <c r="K17">
+        <f>COUNTIF(D1:D635,"0")-I17</f>
+        <v>2</v>
+      </c>
+      <c r="L17">
+        <f>I17+K17</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>45267</v>
       </c>
@@ -42819,7 +42920,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>45267</v>
       </c>
@@ -42839,7 +42940,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>45267</v>
       </c>
@@ -42859,7 +42960,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>45267</v>
       </c>
@@ -42879,7 +42980,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>45267</v>
       </c>
@@ -42899,7 +43000,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>45267</v>
       </c>
@@ -42919,7 +43020,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>45267</v>
       </c>
@@ -42939,7 +43040,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>45267</v>
       </c>
@@ -42959,7 +43060,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>45267</v>
       </c>
@@ -42979,7 +43080,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>45267</v>
       </c>
@@ -42999,7 +43100,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>45267</v>
       </c>
@@ -43019,7 +43120,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>45267</v>
       </c>
@@ -43039,7 +43140,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>45267</v>
       </c>
@@ -43059,7 +43160,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>45267</v>
       </c>
@@ -43079,7 +43180,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>45267</v>
       </c>
@@ -51187,15 +51288,15 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A834D7F-F6A8-4092-9985-A2F842B2FE9D}">
-  <dimension ref="A1:F434"/>
+  <dimension ref="A1:L434"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D434" sqref="B1:D434"/>
+      <selection activeCell="I16" sqref="I16:L17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="1">
         <v>45267</v>
       </c>
@@ -51215,7 +51316,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>45267</v>
       </c>
@@ -51235,7 +51336,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>45267</v>
       </c>
@@ -51255,7 +51356,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>45267</v>
       </c>
@@ -51275,7 +51376,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>45267</v>
       </c>
@@ -51295,7 +51396,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>45267</v>
       </c>
@@ -51315,7 +51416,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>45267</v>
       </c>
@@ -51335,7 +51436,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>45267</v>
       </c>
@@ -51355,7 +51456,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>45267</v>
       </c>
@@ -51375,7 +51476,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>45267</v>
       </c>
@@ -51395,7 +51496,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>45267</v>
       </c>
@@ -51415,7 +51516,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>45267</v>
       </c>
@@ -51435,7 +51536,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>45267</v>
       </c>
@@ -51455,7 +51556,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>45267</v>
       </c>
@@ -51475,7 +51576,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>45267</v>
       </c>
@@ -51495,7 +51596,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>45267</v>
       </c>
@@ -51514,8 +51615,20 @@
       <c r="F16">
         <v>9</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I16" t="s">
+        <v>0</v>
+      </c>
+      <c r="J16" t="s">
+        <v>1</v>
+      </c>
+      <c r="K16" t="s">
+        <v>2</v>
+      </c>
+      <c r="L16" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>45267</v>
       </c>
@@ -51534,8 +51647,24 @@
       <c r="F17">
         <v>9</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I17">
+        <f>COUNTIF(F1:F635,"0")</f>
+        <v>0</v>
+      </c>
+      <c r="J17">
+        <f>COUNTIF(C1:C635,"0")-I17</f>
+        <v>0</v>
+      </c>
+      <c r="K17">
+        <f>COUNTIF(D1:D635,"0")-I17</f>
+        <v>0</v>
+      </c>
+      <c r="L17">
+        <f>I17+K17</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>45267</v>
       </c>
@@ -51555,7 +51684,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>45267</v>
       </c>
@@ -51575,7 +51704,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>45267</v>
       </c>
@@ -51595,7 +51724,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>45267</v>
       </c>
@@ -51615,7 +51744,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>45267</v>
       </c>
@@ -51635,7 +51764,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>45267</v>
       </c>
@@ -51655,7 +51784,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>45267</v>
       </c>
@@ -51675,7 +51804,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>45267</v>
       </c>
@@ -51695,7 +51824,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>45267</v>
       </c>
@@ -51715,7 +51844,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>45267</v>
       </c>
@@ -51735,7 +51864,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>45267</v>
       </c>
@@ -51755,7 +51884,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>45267</v>
       </c>
@@ -51775,7 +51904,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>45267</v>
       </c>
@@ -51795,7 +51924,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>45267</v>
       </c>
@@ -51815,7 +51944,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>45267</v>
       </c>
@@ -59885,7 +60014,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2DA7514-CA06-45AF-A8A5-278A61BFE59C}">
   <dimension ref="A1:F435"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>

</xml_diff>